<commit_message>
relativizando segun el tiempo del experimento
</commit_message>
<xml_diff>
--- a/disenno/disennoREST.xlsx
+++ b/disenno/disennoREST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmora\Desktop\TFG\ESTE_ES_EL_TFG\disenno\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA2DC69-A521-4EA2-8A19-561A467201CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E407C6-4014-4FDC-93BF-BFFB6CE0CC29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12257" yWindow="0" windowWidth="12514" windowHeight="14794" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="74">
   <si>
     <t>Método</t>
   </si>
@@ -245,6 +245,9 @@
   </si>
   <si>
     <t>404: No suitable family found for the provided configuration.</t>
+  </si>
+  <si>
+    <t>/recommendFamily</t>
   </si>
 </sst>
 </file>
@@ -429,26 +432,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -835,19 +838,19 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.75">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="18" t="s">
         <v>20</v>
       </c>
       <c r="F12" s="3" t="s">
@@ -855,39 +858,39 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="58.3">
-      <c r="A13" s="15"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
       <c r="F13" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.75">
-      <c r="A14" s="15"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
       <c r="F14" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.75">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="18" t="s">
         <v>26</v>
       </c>
       <c r="F15" s="3" t="s">
@@ -895,39 +898,39 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="58.3">
-      <c r="A16" s="15"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
       <c r="F16" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="43.75">
-      <c r="A17" s="15"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
       <c r="F17" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.75">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="E18" s="18" t="s">
         <v>30</v>
       </c>
       <c r="F18" s="3" t="s">
@@ -935,11 +938,11 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="58.3">
-      <c r="A19" s="15"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="17"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="18"/>
       <c r="F19" s="3" t="s">
         <v>32</v>
       </c>
@@ -965,19 +968,19 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="43.75">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="17" t="s">
+      <c r="E21" s="18" t="s">
         <v>36</v>
       </c>
       <c r="F21" s="3" t="s">
@@ -985,47 +988,47 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="58.3">
-      <c r="A22" s="15"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
       <c r="F22" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="58.75" thickBot="1">
-      <c r="A23" s="18"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
       <c r="F23" s="6" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:E14"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="E15:E17"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1035,34 +1038,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34229DC1-001C-40B5-B6B8-7068F1C1C81B}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6"/>
   <cols>
-    <col min="2" max="2" width="13.3828125" customWidth="1"/>
+    <col min="2" max="2" width="19.3828125" customWidth="1"/>
     <col min="3" max="3" width="27.921875" customWidth="1"/>
     <col min="6" max="6" width="25.921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="15" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1073,13 +1076,13 @@
       <c r="B2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="18" t="s">
         <v>46</v>
       </c>
       <c r="F2" s="14" t="s">
@@ -1089,9 +1092,9 @@
     <row r="3" spans="1:6" ht="43.75">
       <c r="A3" s="22"/>
       <c r="B3" s="22"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
       <c r="F3" s="14" t="s">
         <v>48</v>
       </c>
@@ -1099,9 +1102,9 @@
     <row r="4" spans="1:6" ht="29.15">
       <c r="A4" s="22"/>
       <c r="B4" s="22"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
       <c r="F4" s="14" t="s">
         <v>49</v>
       </c>
@@ -1113,13 +1116,13 @@
       <c r="B5" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="18" t="s">
         <v>53</v>
       </c>
       <c r="F5" s="14" t="s">
@@ -1129,9 +1132,9 @@
     <row r="6" spans="1:6" ht="43.75">
       <c r="A6" s="22"/>
       <c r="B6" s="22"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
       <c r="F6" s="14" t="s">
         <v>55</v>
       </c>
@@ -1139,9 +1142,9 @@
     <row r="7" spans="1:6" ht="29.15">
       <c r="A7" s="22"/>
       <c r="B7" s="22"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
       <c r="F7" s="14" t="s">
         <v>49</v>
       </c>
@@ -1153,13 +1156,13 @@
       <c r="B8" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="18" t="s">
         <v>58</v>
       </c>
       <c r="F8" s="14" t="s">
@@ -1169,9 +1172,9 @@
     <row r="9" spans="1:6" ht="43.75">
       <c r="A9" s="22"/>
       <c r="B9" s="22"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
       <c r="F9" s="14" t="s">
         <v>55</v>
       </c>
@@ -1179,9 +1182,9 @@
     <row r="10" spans="1:6" ht="29.15">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
       <c r="F10" s="14" t="s">
         <v>49</v>
       </c>
@@ -1193,13 +1196,13 @@
       <c r="B11" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="18" t="s">
         <v>61</v>
       </c>
       <c r="F11" s="14" t="s">
@@ -1209,9 +1212,9 @@
     <row r="12" spans="1:6" ht="29.15">
       <c r="A12" s="22"/>
       <c r="B12" s="22"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="18"/>
       <c r="F12" s="14" t="s">
         <v>63</v>
       </c>
@@ -1223,41 +1226,41 @@
       <c r="B13" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="18" t="s">
         <v>65</v>
       </c>
       <c r="E13" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="F13" s="16"/>
+      <c r="F13" s="17"/>
     </row>
     <row r="14" spans="1:6" ht="102">
       <c r="A14" s="22"/>
       <c r="B14" s="22"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="18"/>
       <c r="E14" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="16"/>
+      <c r="F14" s="17"/>
     </row>
     <row r="15" spans="1:6" ht="29.15">
       <c r="A15" s="22" t="s">
         <v>3</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="18" t="s">
         <v>69</v>
       </c>
       <c r="F15" s="14" t="s">
@@ -1267,9 +1270,9 @@
     <row r="16" spans="1:6" ht="29.15">
       <c r="A16" s="22"/>
       <c r="B16" s="22"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
       <c r="F16" s="14" t="s">
         <v>71</v>
       </c>
@@ -1277,45 +1280,45 @@
     <row r="17" spans="1:6" ht="43.75">
       <c r="A17" s="22"/>
       <c r="B17" s="22"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
       <c r="F17" s="14" t="s">
         <v>72</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="E15:E17"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="F13:F14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>